<commit_message>
just a backup dont push
</commit_message>
<xml_diff>
--- a/Backend/DM_Resource_Plot.xlsx
+++ b/Backend/DM_Resource_Plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MINE\temp\navigated_learning\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D01550-4419-4DAA-8D2E-200666C33697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E580B-3707-4435-9113-751B33E6C38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,7 +863,7 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>